<commit_message>
upgraded pinned-vec and pinned-concurrent-col versions
* Upgraded pinned-vec and pinned-concurrent-col versions.
* boxcar is added to benchmarks.
* Concurrent read & write tests added. Although the api for reading is still unsafe, the tests are not required to be excluded from miri tests. Now all unsafe tests also pass miri tests.
</commit_message>
<xml_diff>
--- a/benches/results/collect.xlsx
+++ b/benches/results/collect.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\uarikan\repos\orx\orx-concurrent-bag\benches\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A16FF053-C2F2-4DA4-9261-54925FF80878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC958CA2-6D84-46CE-8821-BC36BCF20ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="26010" windowHeight="20970" activeTab="1" xr2:uid="{201707E4-C870-4993-88CE-4A7BD9846E2B}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="1" xr2:uid="{201707E4-C870-4993-88CE-4A7BD9846E2B}"/>
   </bookViews>
   <sheets>
     <sheet name="collect_with_push" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="23">
   <si>
     <t>number of elements</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>AppendOnlyVec::push</t>
+  </si>
+  <si>
+    <t>boxcar::Vec::push</t>
   </si>
 </sst>
 </file>
@@ -754,6 +757,79 @@
     <xf numFmtId="9" fontId="4" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -766,79 +842,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1161,10 +1164,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD7FC78D-902C-4DF1-8F50-38A3D8921053}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1175,7 +1178,7 @@
     <col min="5" max="8" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1190,7 +1193,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -1207,12 +1210,9 @@
         <v>6.5256999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>21</v>
-      </c>
-      <c r="C3">
-        <v>32768</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3">
@@ -1222,570 +1222,604 @@
         <v>6.0011000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4">
+        <v>1.6512</v>
+      </c>
+      <c r="G4" s="22">
+        <v>2.1067999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="C4">
-        <v>32768</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4">
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5">
         <v>1.7603</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G5" s="22">
         <v>1.8628</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="C5">
-        <v>32768</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5">
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6">
         <v>1.6412</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G6" s="22">
         <v>3.2086999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="20" t="s">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="20">
-        <v>32768</v>
-      </c>
-      <c r="D6" s="21">
-        <v>0</v>
-      </c>
-      <c r="E6" s="20">
+      <c r="C7" s="20"/>
+      <c r="D7" s="21">
+        <v>0</v>
+      </c>
+      <c r="E7" s="20">
         <v>1.2775000000000001</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="23">
+      <c r="F7" s="20"/>
+      <c r="G7" s="23">
         <v>2.6574</v>
       </c>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B7" t="str">
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" t="str">
         <f>B2</f>
         <v>rayon</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>131072</v>
       </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="24">
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="24">
         <v>6.5094000000000003</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G8" s="22">
         <v>16.443999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B8" t="str">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" t="str">
         <f>B3</f>
         <v>AppendOnlyVec::push</v>
       </c>
-      <c r="C8">
-        <v>131072</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="24">
+      <c r="D9" s="1"/>
+      <c r="E9" s="24">
         <v>24.431999999999999</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G9" s="22">
         <v>24.885000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B9" t="str">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" t="str">
         <f>B4</f>
+        <v>boxcar::Vec::push</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10">
+        <v>6.6147</v>
+      </c>
+      <c r="G10" s="22">
+        <v>12.266999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" t="str">
+        <f>B5</f>
         <v>ConcurrentBag&lt;SplitVec&lt;_, Doubling&gt;&gt;::push</v>
       </c>
-      <c r="C9">
-        <v>131072</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="24">
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="24">
         <v>7.4745999999999997</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G11" s="22">
         <v>8.4802</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B10" t="str">
-        <f>B5</f>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" t="str">
+        <f>B6</f>
         <v>ConcurrentBag&lt;SplitVec&lt;_, Linear&gt;&gt;::push</v>
       </c>
-      <c r="C10">
-        <v>131072</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="24">
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="24">
         <v>6.7279</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G12" s="22">
         <v>12.814</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="20" t="str">
-        <f>B6</f>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="20" t="str">
+        <f>B7</f>
         <v>ConcurrentBag&lt;FixedVec&lt;_&gt;&gt;::push</v>
       </c>
-      <c r="C11" s="20">
-        <v>131072</v>
-      </c>
-      <c r="D11" s="21">
-        <v>0</v>
-      </c>
-      <c r="E11" s="20">
+      <c r="C13" s="20"/>
+      <c r="D13" s="21">
+        <v>0</v>
+      </c>
+      <c r="E13" s="20">
         <v>5.3331999999999997</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20">
+      <c r="F13" s="20"/>
+      <c r="G13" s="20">
         <v>12.677</v>
       </c>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="56"/>
-      <c r="B16" s="56"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="56"/>
-      <c r="B17" s="56"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="56"/>
-      <c r="H17" s="56"/>
-      <c r="I17" s="56"/>
-    </row>
-    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="56"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-    </row>
-    <row r="19" spans="1:9" ht="39.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="56"/>
-      <c r="B19" s="32" t="s">
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
+    </row>
+    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="49"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+    </row>
+    <row r="21" spans="1:9" ht="39.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="49"/>
+      <c r="B21" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="36" t="str">
+      <c r="C21" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="32" t="str">
         <f>D1</f>
         <v>workload</v>
       </c>
-      <c r="E19" s="48" t="s">
+      <c r="E21" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="49"/>
-      <c r="G19" s="40" t="s">
+      <c r="F21" s="51"/>
+      <c r="G21" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="H19" s="28"/>
-      <c r="I19" s="56"/>
-    </row>
-    <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="56"/>
-      <c r="B20" s="33" t="str">
-        <f>B2</f>
+      <c r="H21" s="53"/>
+      <c r="I21" s="49"/>
+    </row>
+    <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="49"/>
+      <c r="B22" s="29" t="str">
+        <f t="shared" ref="B22:C23" si="0">B2</f>
         <v>rayon</v>
       </c>
-      <c r="C20" s="45">
-        <f>C2</f>
+      <c r="C22" s="40">
+        <f t="shared" si="0"/>
         <v>32768</v>
       </c>
-      <c r="D20" s="37">
+      <c r="D22" s="33">
         <f>D2</f>
         <v>0</v>
       </c>
-      <c r="E20" s="50">
-        <f t="shared" ref="E20" si="0">E2</f>
+      <c r="E22" s="43">
+        <f t="shared" ref="E22" si="1">E2</f>
         <v>5.1227999999999998</v>
       </c>
-      <c r="F20" s="51">
-        <f>E20/E$20</f>
+      <c r="F22" s="44">
+        <f>E22/E$22</f>
         <v>1</v>
       </c>
-      <c r="G20" s="41">
-        <f t="shared" ref="G20" si="1">G2</f>
+      <c r="G22" s="36">
+        <f t="shared" ref="G22" si="2">G2</f>
         <v>6.5256999999999996</v>
       </c>
-      <c r="H20" s="25">
-        <f>G20/G$20</f>
+      <c r="H22" s="25">
+        <f>G22/G$22</f>
         <v>1</v>
       </c>
-      <c r="I20" s="56"/>
-    </row>
-    <row r="21" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="56"/>
-      <c r="B21" s="34" t="str">
-        <f>B3</f>
+      <c r="I22" s="49"/>
+    </row>
+    <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="49"/>
+      <c r="B23" s="30" t="str">
+        <f t="shared" si="0"/>
         <v>AppendOnlyVec::push</v>
       </c>
-      <c r="C21" s="46">
-        <f>C3</f>
-        <v>32768</v>
-      </c>
-      <c r="D21" s="38"/>
-      <c r="E21" s="52">
-        <f>E3</f>
+      <c r="C23" s="41"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="45">
+        <f t="shared" ref="E23" si="3">E3</f>
         <v>6.0153999999999996</v>
       </c>
-      <c r="F21" s="53">
-        <f t="shared" ref="F21:F24" si="2">E21/E$20</f>
+      <c r="F23" s="46">
+        <f t="shared" ref="F23:F27" si="4">E23/E$22</f>
         <v>1.1742406496447255</v>
       </c>
-      <c r="G21" s="42">
-        <f>G3</f>
+      <c r="G23" s="37">
+        <f t="shared" ref="G23" si="5">G3</f>
         <v>6.0011000000000001</v>
       </c>
-      <c r="H21" s="26">
-        <f t="shared" ref="H21:H24" si="3">G21/G$20</f>
+      <c r="H23" s="26">
+        <f t="shared" ref="H23:H27" si="6">G23/G$22</f>
         <v>0.91961015676479163</v>
       </c>
-      <c r="I21" s="56"/>
-    </row>
-    <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="56"/>
-      <c r="B22" s="34" t="str">
+      <c r="I23" s="49"/>
+    </row>
+    <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="49"/>
+      <c r="B24" s="30" t="str">
         <f>B4</f>
+        <v>boxcar::Vec::push</v>
+      </c>
+      <c r="C24" s="41"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="45">
+        <f>E4</f>
+        <v>1.6512</v>
+      </c>
+      <c r="F24" s="46">
+        <f t="shared" si="4"/>
+        <v>0.32232372921058799</v>
+      </c>
+      <c r="G24" s="37">
+        <f>G4</f>
+        <v>2.1067999999999998</v>
+      </c>
+      <c r="H24" s="26">
+        <f t="shared" si="6"/>
+        <v>0.3228465911702959</v>
+      </c>
+      <c r="I24" s="49"/>
+    </row>
+    <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="49"/>
+      <c r="B25" s="30" t="str">
+        <f>B5</f>
         <v>ConcurrentBag&lt;SplitVec&lt;_, Doubling&gt;&gt;::push</v>
       </c>
-      <c r="C22" s="46">
-        <f>C4</f>
-        <v>32768</v>
-      </c>
-      <c r="D22" s="38">
-        <f>D4</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="52">
-        <f>E4</f>
+      <c r="C25" s="41"/>
+      <c r="D25" s="34">
+        <f>D5</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="45">
+        <f>E5</f>
         <v>1.7603</v>
       </c>
-      <c r="F22" s="53">
-        <f t="shared" si="2"/>
+      <c r="F25" s="46">
+        <f t="shared" si="4"/>
         <v>0.34362067619270714</v>
       </c>
-      <c r="G22" s="42">
-        <f>G4</f>
+      <c r="G25" s="37">
+        <f>G5</f>
         <v>1.8628</v>
       </c>
-      <c r="H22" s="26">
-        <f t="shared" si="3"/>
+      <c r="H25" s="26">
+        <f t="shared" si="6"/>
         <v>0.28545596640973386</v>
       </c>
-      <c r="I22" s="56"/>
-    </row>
-    <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="56"/>
-      <c r="B23" s="34" t="str">
-        <f>B5</f>
+      <c r="I25" s="49"/>
+    </row>
+    <row r="26" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="49"/>
+      <c r="B26" s="30" t="str">
+        <f>B6</f>
         <v>ConcurrentBag&lt;SplitVec&lt;_, Linear&gt;&gt;::push</v>
       </c>
-      <c r="C23" s="46">
-        <f>C5</f>
-        <v>32768</v>
-      </c>
-      <c r="D23" s="38">
-        <f>D5</f>
-        <v>0</v>
-      </c>
-      <c r="E23" s="52">
-        <f>E5</f>
+      <c r="C26" s="41"/>
+      <c r="D26" s="34">
+        <f>D6</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="45">
+        <f>E6</f>
         <v>1.6412</v>
       </c>
-      <c r="F23" s="53">
-        <f t="shared" si="2"/>
+      <c r="F26" s="46">
+        <f t="shared" si="4"/>
         <v>0.32037167174201608</v>
       </c>
-      <c r="G23" s="42">
-        <f>G5</f>
+      <c r="G26" s="37">
+        <f>G6</f>
         <v>3.2086999999999999</v>
       </c>
-      <c r="H23" s="26">
-        <f t="shared" si="3"/>
+      <c r="H26" s="26">
+        <f t="shared" si="6"/>
         <v>0.49170203962793263</v>
       </c>
-      <c r="I23" s="56"/>
-    </row>
-    <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="56"/>
-      <c r="B24" s="35" t="str">
-        <f>B6</f>
+      <c r="I26" s="49"/>
+    </row>
+    <row r="27" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="49"/>
+      <c r="B27" s="31" t="str">
+        <f>B7</f>
         <v>ConcurrentBag&lt;FixedVec&lt;_&gt;&gt;::push</v>
       </c>
-      <c r="C24" s="47">
-        <f>C6</f>
-        <v>32768</v>
-      </c>
-      <c r="D24" s="39">
-        <f>D6</f>
-        <v>0</v>
-      </c>
-      <c r="E24" s="54">
-        <f>E6</f>
+      <c r="C27" s="42"/>
+      <c r="D27" s="35">
+        <f>D7</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="47">
+        <f>E7</f>
         <v>1.2775000000000001</v>
       </c>
-      <c r="F24" s="55">
-        <f t="shared" si="2"/>
+      <c r="F27" s="48">
+        <f t="shared" si="4"/>
         <v>0.24937534161005703</v>
       </c>
-      <c r="G24" s="43">
-        <f>G6</f>
+      <c r="G27" s="38">
+        <f>G7</f>
         <v>2.6574</v>
       </c>
-      <c r="H24" s="27">
-        <f t="shared" si="3"/>
+      <c r="H27" s="27">
+        <f t="shared" si="6"/>
         <v>0.40722068130622002</v>
       </c>
-      <c r="I24" s="56"/>
-    </row>
-    <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="56"/>
-      <c r="B25" s="33" t="str">
-        <f>B7</f>
+      <c r="I27" s="49"/>
+    </row>
+    <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="49"/>
+      <c r="B28" s="29" t="str">
+        <f>B8</f>
         <v>rayon</v>
       </c>
-      <c r="C25" s="45">
-        <f>C7</f>
-        <v>131072</v>
-      </c>
-      <c r="D25" s="37">
-        <f>D7</f>
-        <v>0</v>
-      </c>
-      <c r="E25" s="50">
-        <f>E7</f>
-        <v>6.5094000000000003</v>
-      </c>
-      <c r="F25" s="51">
-        <f>E25/E$25</f>
-        <v>1</v>
-      </c>
-      <c r="G25" s="41">
-        <f>G7</f>
-        <v>16.443999999999999</v>
-      </c>
-      <c r="H25" s="25">
-        <f>G25/G$25</f>
-        <v>1</v>
-      </c>
-      <c r="I25" s="56"/>
-    </row>
-    <row r="26" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="56"/>
-      <c r="B26" s="34" t="str">
-        <f>B8</f>
-        <v>AppendOnlyVec::push</v>
-      </c>
-      <c r="C26" s="46">
+      <c r="C28" s="40">
         <f>C8</f>
         <v>131072</v>
       </c>
-      <c r="D26" s="38"/>
-      <c r="E26" s="52">
+      <c r="D28" s="33">
+        <f>D8</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="43">
         <f>E8</f>
+        <v>6.5094000000000003</v>
+      </c>
+      <c r="F28" s="44">
+        <f>E28/E$28</f>
+        <v>1</v>
+      </c>
+      <c r="G28" s="36">
+        <f>G8</f>
+        <v>16.443999999999999</v>
+      </c>
+      <c r="H28" s="25">
+        <f>G28/G$28</f>
+        <v>1</v>
+      </c>
+      <c r="I28" s="49"/>
+    </row>
+    <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="49"/>
+      <c r="B29" s="30" t="str">
+        <f>B9</f>
+        <v>AppendOnlyVec::push</v>
+      </c>
+      <c r="C29" s="41"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="45">
+        <f>E9</f>
         <v>24.431999999999999</v>
       </c>
-      <c r="F26" s="53">
-        <f t="shared" ref="F26:F29" si="4">E26/E$25</f>
+      <c r="F29" s="46">
+        <f t="shared" ref="F29:F33" si="7">E29/E$28</f>
         <v>3.7533413217808089</v>
       </c>
-      <c r="G26" s="42">
-        <f>G8</f>
+      <c r="G29" s="37">
+        <f>G9</f>
         <v>24.885000000000002</v>
       </c>
-      <c r="H26" s="26">
-        <f t="shared" ref="H26:H29" si="5">G26/G$25</f>
+      <c r="H29" s="26">
+        <f t="shared" ref="H29:H33" si="8">G29/G$28</f>
         <v>1.5133179275115545</v>
       </c>
-      <c r="I26" s="56"/>
-    </row>
-    <row r="27" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="56"/>
-      <c r="B27" s="34" t="str">
-        <f>B9</f>
+      <c r="I29" s="49"/>
+    </row>
+    <row r="30" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="49"/>
+      <c r="B30" s="30" t="str">
+        <f>B10</f>
+        <v>boxcar::Vec::push</v>
+      </c>
+      <c r="C30" s="41"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="45">
+        <f>E10</f>
+        <v>6.6147</v>
+      </c>
+      <c r="F30" s="46">
+        <f t="shared" si="7"/>
+        <v>1.0161766061388147</v>
+      </c>
+      <c r="G30" s="37">
+        <f>G10</f>
+        <v>12.266999999999999</v>
+      </c>
+      <c r="H30" s="26">
+        <f t="shared" si="8"/>
+        <v>0.7459863780102165</v>
+      </c>
+      <c r="I30" s="49"/>
+    </row>
+    <row r="31" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="49"/>
+      <c r="B31" s="30" t="str">
+        <f>B11</f>
         <v>ConcurrentBag&lt;SplitVec&lt;_, Doubling&gt;&gt;::push</v>
       </c>
-      <c r="C27" s="46">
-        <f>C9</f>
-        <v>131072</v>
-      </c>
-      <c r="D27" s="38">
-        <f>D9</f>
-        <v>0</v>
-      </c>
-      <c r="E27" s="52">
-        <f>E9</f>
+      <c r="C31" s="41"/>
+      <c r="D31" s="34">
+        <f>D11</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="45">
+        <f>E11</f>
         <v>7.4745999999999997</v>
       </c>
-      <c r="F27" s="53">
-        <f t="shared" si="4"/>
+      <c r="F31" s="46">
+        <f t="shared" si="7"/>
         <v>1.1482778750729712</v>
       </c>
-      <c r="G27" s="42">
-        <f>G9</f>
+      <c r="G31" s="37">
+        <f>G11</f>
         <v>8.4802</v>
       </c>
-      <c r="H27" s="26">
-        <f t="shared" si="5"/>
+      <c r="H31" s="26">
+        <f t="shared" si="8"/>
         <v>0.51570177572366827</v>
       </c>
-      <c r="I27" s="56"/>
-    </row>
-    <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="56"/>
-      <c r="B28" s="34" t="str">
-        <f>B10</f>
+      <c r="I31" s="49"/>
+    </row>
+    <row r="32" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="49"/>
+      <c r="B32" s="30" t="str">
+        <f>B12</f>
         <v>ConcurrentBag&lt;SplitVec&lt;_, Linear&gt;&gt;::push</v>
       </c>
-      <c r="C28" s="46">
-        <f>C10</f>
-        <v>131072</v>
-      </c>
-      <c r="D28" s="38">
-        <f>D10</f>
-        <v>0</v>
-      </c>
-      <c r="E28" s="52">
-        <f>E10</f>
+      <c r="C32" s="41"/>
+      <c r="D32" s="34">
+        <f>D12</f>
+        <v>0</v>
+      </c>
+      <c r="E32" s="45">
+        <f>E12</f>
         <v>6.7279</v>
       </c>
-      <c r="F28" s="53">
-        <f t="shared" si="4"/>
+      <c r="F32" s="46">
+        <f t="shared" si="7"/>
         <v>1.0335668417980151</v>
       </c>
-      <c r="G28" s="42">
-        <f>G10</f>
+      <c r="G32" s="37">
+        <f>G12</f>
         <v>12.814</v>
       </c>
-      <c r="H28" s="26">
-        <f t="shared" si="5"/>
+      <c r="H32" s="26">
+        <f t="shared" si="8"/>
         <v>0.77925079056190716</v>
       </c>
-      <c r="I28" s="56"/>
-    </row>
-    <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="56"/>
-      <c r="B29" s="35" t="str">
-        <f>B11</f>
+      <c r="I32" s="49"/>
+    </row>
+    <row r="33" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="49"/>
+      <c r="B33" s="31" t="str">
+        <f>B13</f>
         <v>ConcurrentBag&lt;FixedVec&lt;_&gt;&gt;::push</v>
       </c>
-      <c r="C29" s="47">
-        <f>C11</f>
-        <v>131072</v>
-      </c>
-      <c r="D29" s="39">
-        <f>D11</f>
-        <v>0</v>
-      </c>
-      <c r="E29" s="54">
-        <f>E11</f>
+      <c r="C33" s="42"/>
+      <c r="D33" s="35">
+        <f>D13</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="47">
+        <f>E13</f>
         <v>5.3331999999999997</v>
       </c>
-      <c r="F29" s="55">
-        <f t="shared" si="4"/>
+      <c r="F33" s="48">
+        <f t="shared" si="7"/>
         <v>0.81930746305343038</v>
       </c>
-      <c r="G29" s="43">
-        <f>G11</f>
+      <c r="G33" s="38">
+        <f>G13</f>
         <v>12.677</v>
       </c>
-      <c r="H29" s="27">
-        <f t="shared" si="5"/>
+      <c r="H33" s="27">
+        <f t="shared" si="8"/>
         <v>0.77091948431038682</v>
       </c>
-      <c r="I29" s="56"/>
-    </row>
-    <row r="30" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="56"/>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="56"/>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="56"/>
-      <c r="B32" s="56"/>
-      <c r="C32" s="56"/>
-      <c r="D32" s="56"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="56"/>
-      <c r="G32" s="56"/>
-      <c r="H32" s="56"/>
-      <c r="I32" s="56"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="56"/>
-      <c r="B33" s="56"/>
-      <c r="C33" s="56"/>
-      <c r="D33" s="56"/>
-      <c r="E33" s="56"/>
-      <c r="F33" s="56"/>
-      <c r="G33" s="56"/>
-      <c r="H33" s="56"/>
-      <c r="I33" s="56"/>
+      <c r="I33" s="49"/>
+    </row>
+    <row r="34" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="49"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="49"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="49"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="49"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="49"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
   </mergeCells>
-  <conditionalFormatting sqref="F20:F24">
+  <conditionalFormatting sqref="F22:F27">
     <cfRule type="dataBar" priority="4">
       <dataBar showValue="0">
         <cfvo type="min"/>
@@ -1799,7 +1833,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F25:F29">
+  <conditionalFormatting sqref="F28:F33">
     <cfRule type="dataBar" priority="3">
       <dataBar showValue="0">
         <cfvo type="min"/>
@@ -1813,7 +1847,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H20:H24">
+  <conditionalFormatting sqref="H22:H27">
     <cfRule type="dataBar" priority="2">
       <dataBar showValue="0">
         <cfvo type="min"/>
@@ -1827,7 +1861,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H25:H29">
+  <conditionalFormatting sqref="H28:H33">
     <cfRule type="dataBar" priority="1">
       <dataBar showValue="0">
         <cfvo type="min"/>
@@ -1844,7 +1878,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="F27:F29 F22:F25 F20" formula="1"/>
+    <ignoredError sqref="F31:F33 F25:F28 F22" formula="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -1858,7 +1892,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F20:F24</xm:sqref>
+          <xm:sqref>F22:F27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{E9B70DED-250E-46E6-A5C7-D5F48F2D6F77}">
@@ -1869,7 +1903,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F25:F29</xm:sqref>
+          <xm:sqref>F28:F33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{B022FDA3-7EBB-4DC4-A3A9-6D235CB84EE1}">
@@ -1880,7 +1914,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H20:H24</xm:sqref>
+          <xm:sqref>H22:H27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{01B817C0-39B1-4552-A0FE-5DFFA6937FE7}">
@@ -1891,7 +1925,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H25:H29</xm:sqref>
+          <xm:sqref>H28:H33</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1901,10 +1935,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCAC745C-D468-49EC-93AB-3CA0AF648CD4}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1951,555 +1985,622 @@
       <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="C3">
-        <v>32768</v>
-      </c>
       <c r="D3" s="1"/>
       <c r="E3">
-        <v>6.5103999999999997</v>
-      </c>
-      <c r="G3" s="22">
-        <v>6.4617000000000004</v>
+        <f>collect_with_push!E3</f>
+        <v>6.0153999999999996</v>
+      </c>
+      <c r="G3">
+        <f>collect_with_push!G3</f>
+        <v>6.0011000000000001</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4">
-        <v>32768</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D4" s="1"/>
       <c r="E4">
-        <v>0.16238</v>
-      </c>
-      <c r="G4" s="22">
-        <v>0.48294999999999999</v>
+        <f>collect_with_push!E4</f>
+        <v>1.6512</v>
+      </c>
+      <c r="G4">
+        <f>collect_with_push!G4</f>
+        <v>2.1067999999999998</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0.16238</v>
+      </c>
+      <c r="G5" s="22">
+        <v>0.48294999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="C5">
-        <v>32768</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5">
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6">
         <v>0.15695000000000001</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G6" s="22">
         <v>0.42180000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="20" t="s">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="20">
-        <v>32768</v>
-      </c>
-      <c r="D6" s="21">
-        <v>0</v>
-      </c>
-      <c r="E6" s="20">
+      <c r="C7" s="20"/>
+      <c r="D7" s="21">
+        <v>0</v>
+      </c>
+      <c r="E7" s="20">
         <v>0.15395</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="23">
+      <c r="F7" s="20"/>
+      <c r="G7" s="23">
         <v>0.43234</v>
       </c>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" t="str">
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" t="str">
         <f>B2</f>
         <v>rayon</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>131072</v>
       </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7">
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8">
         <v>6.7740999999999998</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G8" s="22">
         <v>16.777999999999999</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" t="str">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" t="str">
         <f>B3</f>
         <v>AppendOnlyVec::push</v>
       </c>
-      <c r="C8">
-        <v>131072</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8">
-        <v>25.175999999999998</v>
-      </c>
-      <c r="G8" s="22">
-        <v>25.814</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" t="str">
-        <f>B4</f>
-        <v>ConcurrentBag&lt;SplitVec&lt;_, Doubling&gt;&gt;::extend</v>
-      </c>
-      <c r="C9">
-        <v>131072</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
+      <c r="D9" s="1"/>
       <c r="E9">
-        <v>0.23336000000000001</v>
-      </c>
-      <c r="G9" s="22">
-        <v>1.6212</v>
+        <f>collect_with_push!E9</f>
+        <v>24.431999999999999</v>
+      </c>
+      <c r="G9">
+        <f>collect_with_push!G9</f>
+        <v>24.885000000000002</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" t="str">
-        <f>B5</f>
-        <v>ConcurrentBag&lt;SplitVec&lt;_, Linear&gt;&gt;::extend</v>
-      </c>
-      <c r="C10">
-        <v>131072</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
+        <f>B4</f>
+        <v>boxcar::Vec::push</v>
+      </c>
+      <c r="D10" s="1"/>
       <c r="E10">
-        <v>0.21779999999999999</v>
-      </c>
-      <c r="G10" s="22">
-        <v>1.3922000000000001</v>
+        <f>collect_with_push!E10</f>
+        <v>6.6147</v>
+      </c>
+      <c r="G10">
+        <f>collect_with_push!G10</f>
+        <v>12.266999999999999</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" t="str">
+        <f>B5</f>
+        <v>ConcurrentBag&lt;SplitVec&lt;_, Doubling&gt;&gt;::extend</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0.23336000000000001</v>
+      </c>
+      <c r="G11" s="22">
+        <v>1.6212</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" t="str">
         <f>B6</f>
+        <v>ConcurrentBag&lt;SplitVec&lt;_, Linear&gt;&gt;::extend</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0.21779999999999999</v>
+      </c>
+      <c r="G12" s="22">
+        <v>1.3922000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13" t="str">
+        <f>B7</f>
         <v>ConcurrentBag&lt;FixedVec&lt;_&gt;&gt;::extend</v>
       </c>
-      <c r="C11" s="20">
-        <v>131072</v>
-      </c>
-      <c r="D11" s="21">
-        <v>0</v>
-      </c>
-      <c r="E11" s="20">
+      <c r="C13" s="20"/>
+      <c r="D13" s="21">
+        <v>0</v>
+      </c>
+      <c r="E13" s="20">
         <v>0.21037</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20">
+      <c r="F13" s="20"/>
+      <c r="G13" s="20">
         <v>3.5659999999999998</v>
       </c>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="56"/>
-      <c r="B17" s="56"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="56"/>
-      <c r="H17" s="56"/>
-      <c r="I17" s="56"/>
-    </row>
-    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="56"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-    </row>
-    <row r="19" spans="1:9" ht="39.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="56"/>
-      <c r="B19" s="32" t="s">
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
+    </row>
+    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="49"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+    </row>
+    <row r="21" spans="1:9" ht="39.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="49"/>
+      <c r="B21" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="36" t="str">
+      <c r="C21" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="32" t="str">
         <f>D1</f>
         <v>workload</v>
       </c>
-      <c r="E19" s="48" t="s">
+      <c r="E21" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="49"/>
-      <c r="G19" s="40" t="s">
+      <c r="F21" s="51"/>
+      <c r="G21" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="H19" s="28"/>
-      <c r="I19" s="56"/>
-    </row>
-    <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="56"/>
-      <c r="B20" s="33" t="str">
+      <c r="H21" s="53"/>
+      <c r="I21" s="49"/>
+    </row>
+    <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="49"/>
+      <c r="B22" s="29" t="str">
         <f>B2</f>
         <v>rayon</v>
       </c>
-      <c r="C20" s="45">
+      <c r="C22" s="40">
         <f>C2</f>
         <v>32768</v>
       </c>
-      <c r="D20" s="37">
+      <c r="D22" s="33">
         <f>D2</f>
         <v>0</v>
       </c>
-      <c r="E20" s="50">
-        <f t="shared" ref="E20" si="0">E2</f>
+      <c r="E22" s="43">
+        <f>E2</f>
         <v>5.1844999999999999</v>
       </c>
-      <c r="F20" s="51">
-        <f>E20/E$20</f>
+      <c r="F22" s="44">
+        <f>E22/E$22</f>
         <v>1</v>
       </c>
-      <c r="G20" s="41">
-        <f t="shared" ref="G20" si="1">G2</f>
+      <c r="G22" s="36">
+        <f>G2</f>
         <v>6.0444000000000004</v>
       </c>
-      <c r="H20" s="25">
-        <f>G20/G$20</f>
+      <c r="H22" s="25">
+        <f>G22/G$22</f>
         <v>1</v>
       </c>
-      <c r="I20" s="56"/>
-    </row>
-    <row r="21" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="56"/>
-      <c r="B21" s="34" t="str">
+      <c r="I22" s="49"/>
+    </row>
+    <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="49"/>
+      <c r="B23" s="30" t="str">
         <f>B3</f>
         <v>AppendOnlyVec::push</v>
       </c>
-      <c r="C21" s="46">
-        <f>C3</f>
-        <v>32768</v>
-      </c>
-      <c r="D21" s="38">
+      <c r="C23" s="41"/>
+      <c r="D23" s="34">
         <f>D3</f>
         <v>0</v>
       </c>
-      <c r="E21" s="52">
-        <f>E3</f>
-        <v>6.5103999999999997</v>
-      </c>
-      <c r="F21" s="53">
-        <f t="shared" ref="F21:F24" si="2">E21/E$20</f>
-        <v>1.2557430803356158</v>
-      </c>
-      <c r="G21" s="42">
-        <f>G3</f>
-        <v>6.4617000000000004</v>
-      </c>
-      <c r="H21" s="26">
-        <f t="shared" ref="H21:H24" si="3">G21/G$20</f>
-        <v>1.0690391105816954</v>
-      </c>
-      <c r="I21" s="56"/>
-    </row>
-    <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="56"/>
-      <c r="B22" s="34" t="str">
+      <c r="E23" s="45">
+        <f t="shared" ref="E23" si="0">E3</f>
+        <v>6.0153999999999996</v>
+      </c>
+      <c r="F23" s="46">
+        <f t="shared" ref="F23:F27" si="1">E23/E$22</f>
+        <v>1.1602661780306682</v>
+      </c>
+      <c r="G23" s="37">
+        <f t="shared" ref="G23" si="2">G3</f>
+        <v>6.0011000000000001</v>
+      </c>
+      <c r="H23" s="26">
+        <f t="shared" ref="H23:H27" si="3">G23/G$22</f>
+        <v>0.99283634438488511</v>
+      </c>
+      <c r="I23" s="49"/>
+    </row>
+    <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="49"/>
+      <c r="B24" s="30" t="str">
         <f>B4</f>
+        <v>boxcar::Vec::push</v>
+      </c>
+      <c r="C24" s="41"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="45">
+        <f>E4</f>
+        <v>1.6512</v>
+      </c>
+      <c r="F24" s="46">
+        <f t="shared" si="1"/>
+        <v>0.31848780017359435</v>
+      </c>
+      <c r="G24" s="37">
+        <f>G4</f>
+        <v>2.1067999999999998</v>
+      </c>
+      <c r="H24" s="26">
+        <f t="shared" si="3"/>
+        <v>0.34855403348554026</v>
+      </c>
+      <c r="I24" s="49"/>
+    </row>
+    <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="49"/>
+      <c r="B25" s="30" t="str">
+        <f>B5</f>
         <v>ConcurrentBag&lt;SplitVec&lt;_, Doubling&gt;&gt;::extend</v>
       </c>
-      <c r="C22" s="46">
-        <f>C4</f>
-        <v>32768</v>
-      </c>
-      <c r="D22" s="38">
-        <f>D4</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="52">
-        <f>E4</f>
+      <c r="C25" s="41"/>
+      <c r="D25" s="34">
+        <f>D5</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="45">
+        <f>E5</f>
         <v>0.16238</v>
       </c>
-      <c r="F22" s="53">
-        <f t="shared" si="2"/>
+      <c r="F25" s="46">
+        <f t="shared" si="1"/>
         <v>3.1320281608641143E-2</v>
       </c>
-      <c r="G22" s="42">
-        <f>G4</f>
+      <c r="G25" s="37">
+        <f>G5</f>
         <v>0.48294999999999999</v>
       </c>
-      <c r="H22" s="26">
+      <c r="H25" s="26">
         <f t="shared" si="3"/>
         <v>7.9900403679438806E-2</v>
       </c>
-      <c r="I22" s="56"/>
-    </row>
-    <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="56"/>
-      <c r="B23" s="34" t="str">
-        <f>B5</f>
+      <c r="I25" s="49"/>
+    </row>
+    <row r="26" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="49"/>
+      <c r="B26" s="30" t="str">
+        <f>B6</f>
         <v>ConcurrentBag&lt;SplitVec&lt;_, Linear&gt;&gt;::extend</v>
       </c>
-      <c r="C23" s="46">
-        <f>C5</f>
-        <v>32768</v>
-      </c>
-      <c r="D23" s="38">
-        <f>D5</f>
-        <v>0</v>
-      </c>
-      <c r="E23" s="52">
-        <f>E5</f>
+      <c r="C26" s="41"/>
+      <c r="D26" s="34">
+        <f>D6</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="45">
+        <f>E6</f>
         <v>0.15695000000000001</v>
       </c>
-      <c r="F23" s="53">
-        <f t="shared" si="2"/>
+      <c r="F26" s="46">
+        <f t="shared" si="1"/>
         <v>3.0272928922750509E-2</v>
       </c>
-      <c r="G23" s="42">
-        <f>G5</f>
+      <c r="G26" s="37">
+        <f>G6</f>
         <v>0.42180000000000001</v>
       </c>
-      <c r="H23" s="26">
+      <c r="H26" s="26">
         <f t="shared" si="3"/>
         <v>6.9783601350009924E-2</v>
       </c>
-      <c r="I23" s="56"/>
-    </row>
-    <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="56"/>
-      <c r="B24" s="35" t="str">
-        <f>B6</f>
+      <c r="I26" s="49"/>
+    </row>
+    <row r="27" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="49"/>
+      <c r="B27" s="31" t="str">
+        <f>B7</f>
         <v>ConcurrentBag&lt;FixedVec&lt;_&gt;&gt;::extend</v>
       </c>
-      <c r="C24" s="47">
-        <f>C6</f>
-        <v>32768</v>
-      </c>
-      <c r="D24" s="39">
-        <f>D6</f>
-        <v>0</v>
-      </c>
-      <c r="E24" s="54">
-        <f>E6</f>
+      <c r="C27" s="42"/>
+      <c r="D27" s="35">
+        <f>D7</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="47">
+        <f>E7</f>
         <v>0.15395</v>
       </c>
-      <c r="F24" s="55">
-        <f t="shared" si="2"/>
+      <c r="F27" s="48">
+        <f t="shared" si="1"/>
         <v>2.969428102999325E-2</v>
       </c>
-      <c r="G24" s="43">
-        <f>G6</f>
+      <c r="G27" s="38">
+        <f>G7</f>
         <v>0.43234</v>
       </c>
-      <c r="H24" s="27">
+      <c r="H27" s="27">
         <f t="shared" si="3"/>
         <v>7.152736417179538E-2</v>
       </c>
-      <c r="I24" s="56"/>
-    </row>
-    <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="56"/>
-      <c r="B25" s="33" t="str">
-        <f>B7</f>
+      <c r="I27" s="49"/>
+    </row>
+    <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="49"/>
+      <c r="B28" s="29" t="str">
+        <f>B8</f>
         <v>rayon</v>
       </c>
-      <c r="C25" s="45">
-        <f>C7</f>
-        <v>131072</v>
-      </c>
-      <c r="D25" s="37">
-        <f>D7</f>
-        <v>0</v>
-      </c>
-      <c r="E25" s="50">
-        <f>E7</f>
-        <v>6.7740999999999998</v>
-      </c>
-      <c r="F25" s="51">
-        <f>E25/E$25</f>
-        <v>1</v>
-      </c>
-      <c r="G25" s="41">
-        <f>G7</f>
-        <v>16.777999999999999</v>
-      </c>
-      <c r="H25" s="25">
-        <f>G25/G$25</f>
-        <v>1</v>
-      </c>
-      <c r="I25" s="56"/>
-    </row>
-    <row r="26" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="56"/>
-      <c r="B26" s="34" t="str">
-        <f>B8</f>
-        <v>AppendOnlyVec::push</v>
-      </c>
-      <c r="C26" s="46">
+      <c r="C28" s="40">
         <f>C8</f>
         <v>131072</v>
       </c>
-      <c r="D26" s="38">
+      <c r="D28" s="33">
         <f>D8</f>
         <v>0</v>
       </c>
-      <c r="E26" s="52">
+      <c r="E28" s="43">
         <f>E8</f>
-        <v>25.175999999999998</v>
-      </c>
-      <c r="F26" s="53">
-        <f t="shared" ref="F26:F29" si="4">E26/E$25</f>
-        <v>3.7165084660692931</v>
-      </c>
-      <c r="G26" s="42">
+        <v>6.7740999999999998</v>
+      </c>
+      <c r="F28" s="44">
+        <f>E28/E$28</f>
+        <v>1</v>
+      </c>
+      <c r="G28" s="36">
         <f>G8</f>
-        <v>25.814</v>
-      </c>
-      <c r="H26" s="26">
-        <f t="shared" ref="H26:H29" si="5">G26/G$25</f>
-        <v>1.5385624031469782</v>
-      </c>
-      <c r="I26" s="56"/>
-    </row>
-    <row r="27" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="56"/>
-      <c r="B27" s="34" t="str">
+        <v>16.777999999999999</v>
+      </c>
+      <c r="H28" s="25">
+        <f>G28/G$28</f>
+        <v>1</v>
+      </c>
+      <c r="I28" s="49"/>
+    </row>
+    <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="49"/>
+      <c r="B29" s="30" t="str">
         <f>B9</f>
+        <v>AppendOnlyVec::push</v>
+      </c>
+      <c r="C29" s="41"/>
+      <c r="D29" s="34">
+        <f>D9</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="45">
+        <f>E9</f>
+        <v>24.431999999999999</v>
+      </c>
+      <c r="F29" s="46">
+        <f t="shared" ref="F29:F33" si="4">E29/E$28</f>
+        <v>3.6066783779395046</v>
+      </c>
+      <c r="G29" s="37">
+        <f>G9</f>
+        <v>24.885000000000002</v>
+      </c>
+      <c r="H29" s="26">
+        <f t="shared" ref="H29:H33" si="5">G29/G$28</f>
+        <v>1.4831922755989988</v>
+      </c>
+      <c r="I29" s="49"/>
+    </row>
+    <row r="30" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="49"/>
+      <c r="B30" s="30" t="str">
+        <f>B10</f>
+        <v>boxcar::Vec::push</v>
+      </c>
+      <c r="C30" s="41"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="45">
+        <f>E10</f>
+        <v>6.6147</v>
+      </c>
+      <c r="F30" s="46">
+        <f t="shared" si="4"/>
+        <v>0.97646919886036521</v>
+      </c>
+      <c r="G30" s="37">
+        <f>G10</f>
+        <v>12.266999999999999</v>
+      </c>
+      <c r="H30" s="26">
+        <f t="shared" si="5"/>
+        <v>0.73113601144355711</v>
+      </c>
+      <c r="I30" s="49"/>
+    </row>
+    <row r="31" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="49"/>
+      <c r="B31" s="30" t="str">
+        <f>B11</f>
         <v>ConcurrentBag&lt;SplitVec&lt;_, Doubling&gt;&gt;::extend</v>
       </c>
-      <c r="C27" s="46">
-        <f>C9</f>
-        <v>131072</v>
-      </c>
-      <c r="D27" s="38">
-        <f>D9</f>
-        <v>0</v>
-      </c>
-      <c r="E27" s="52">
-        <f>E9</f>
+      <c r="C31" s="41"/>
+      <c r="D31" s="34">
+        <f>D11</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="45">
+        <f>E11</f>
         <v>0.23336000000000001</v>
       </c>
-      <c r="F27" s="53">
+      <c r="F31" s="46">
         <f t="shared" si="4"/>
         <v>3.4448856674687417E-2</v>
       </c>
-      <c r="G27" s="42">
-        <f>G9</f>
+      <c r="G31" s="37">
+        <f>G11</f>
         <v>1.6212</v>
       </c>
-      <c r="H27" s="26">
+      <c r="H31" s="26">
         <f t="shared" si="5"/>
         <v>9.6626534747884144E-2</v>
       </c>
-      <c r="I27" s="56"/>
-    </row>
-    <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="56"/>
-      <c r="B28" s="34" t="str">
-        <f>B10</f>
+      <c r="I31" s="49"/>
+    </row>
+    <row r="32" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="49"/>
+      <c r="B32" s="30" t="str">
+        <f>B12</f>
         <v>ConcurrentBag&lt;SplitVec&lt;_, Linear&gt;&gt;::extend</v>
       </c>
-      <c r="C28" s="46">
-        <f>C10</f>
-        <v>131072</v>
-      </c>
-      <c r="D28" s="38">
-        <f>D10</f>
-        <v>0</v>
-      </c>
-      <c r="E28" s="52">
-        <f>E10</f>
+      <c r="C32" s="41"/>
+      <c r="D32" s="34">
+        <f>D12</f>
+        <v>0</v>
+      </c>
+      <c r="E32" s="45">
+        <f>E12</f>
         <v>0.21779999999999999</v>
       </c>
-      <c r="F28" s="53">
+      <c r="F32" s="46">
         <f t="shared" si="4"/>
         <v>3.2151872573478395E-2</v>
       </c>
-      <c r="G28" s="42">
-        <f>G10</f>
+      <c r="G32" s="37">
+        <f>G12</f>
         <v>1.3922000000000001</v>
       </c>
-      <c r="H28" s="26">
+      <c r="H32" s="26">
         <f t="shared" si="5"/>
         <v>8.2977708904517833E-2</v>
       </c>
-      <c r="I28" s="56"/>
-    </row>
-    <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="56"/>
-      <c r="B29" s="35" t="str">
-        <f>B11</f>
+      <c r="I32" s="49"/>
+    </row>
+    <row r="33" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="49"/>
+      <c r="B33" s="31" t="str">
+        <f>B13</f>
         <v>ConcurrentBag&lt;FixedVec&lt;_&gt;&gt;::extend</v>
       </c>
-      <c r="C29" s="47">
-        <f>C11</f>
-        <v>131072</v>
-      </c>
-      <c r="D29" s="39">
-        <f>D11</f>
-        <v>0</v>
-      </c>
-      <c r="E29" s="54">
-        <f>E11</f>
+      <c r="C33" s="42"/>
+      <c r="D33" s="35">
+        <f>D13</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="47">
+        <f>E13</f>
         <v>0.21037</v>
       </c>
-      <c r="F29" s="55">
+      <c r="F33" s="48">
         <f t="shared" si="4"/>
         <v>3.1055047903042473E-2</v>
       </c>
-      <c r="G29" s="43">
-        <f>G11</f>
+      <c r="G33" s="38">
+        <f>G13</f>
         <v>3.5659999999999998</v>
       </c>
-      <c r="H29" s="27">
+      <c r="H33" s="27">
         <f t="shared" si="5"/>
         <v>0.21254023125521518</v>
       </c>
-      <c r="I29" s="56"/>
-    </row>
-    <row r="30" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="56"/>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="56"/>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
+      <c r="I33" s="49"/>
+    </row>
+    <row r="34" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="49"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="49"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
   </mergeCells>
-  <conditionalFormatting sqref="F20:F24">
-    <cfRule type="dataBar" priority="4">
+  <conditionalFormatting sqref="F28:F33">
+    <cfRule type="dataBar" priority="9">
+      <dataBar showValue="0">
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF3300"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{1A28700B-E465-4EB4-8FEE-7612FD1016C3}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H28:H33">
+    <cfRule type="dataBar" priority="11">
+      <dataBar showValue="0">
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF3300"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{860C8C02-C98D-4E5B-AE47-C78A98AE937F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22:F27">
+    <cfRule type="dataBar" priority="12">
       <dataBar showValue="0">
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2512,22 +2613,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F25:F29">
-    <cfRule type="dataBar" priority="3">
-      <dataBar showValue="0">
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF3300"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{1A28700B-E465-4EB4-8FEE-7612FD1016C3}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H20:H24">
-    <cfRule type="dataBar" priority="2">
+  <conditionalFormatting sqref="H22:H27">
+    <cfRule type="dataBar" priority="14">
       <dataBar showValue="0">
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2540,28 +2627,36 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H25:H29">
-    <cfRule type="dataBar" priority="1">
-      <dataBar showValue="0">
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF3300"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{860C8C02-C98D-4E5B-AE47-C78A98AE937F}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="F27:F29 F22:F25 F20" formula="1"/>
+    <ignoredError sqref="F31:F33 F25:F28 F22" formula="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{1A28700B-E465-4EB4-8FEE-7612FD1016C3}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F28:F33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{860C8C02-C98D-4E5B-AE47-C78A98AE937F}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H28:H33</xm:sqref>
+        </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{2957D239-BCD4-45F5-8859-242251531A0B}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
@@ -2571,18 +2666,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F20:F24</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{1A28700B-E465-4EB4-8FEE-7612FD1016C3}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>F25:F29</xm:sqref>
+          <xm:sqref>F22:F27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{EFD277FB-0233-4310-96A1-652DC21423DE}">
@@ -2593,18 +2677,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H20:H24</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{860C8C02-C98D-4E5B-AE47-C78A98AE937F}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>H25:H29</xm:sqref>
+          <xm:sqref>H22:H27</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2616,7 +2689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF97F42C-248E-4367-AF13-B78D57BAABDB}">
   <dimension ref="B1:I58"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
@@ -3085,14 +3158,14 @@
         <f>D1</f>
         <v>workload</v>
       </c>
-      <c r="E34" s="29" t="s">
+      <c r="E34" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="F34" s="30"/>
-      <c r="G34" s="29" t="s">
+      <c r="F34" s="55"/>
+      <c r="G34" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="H34" s="31"/>
+      <c r="H34" s="56"/>
     </row>
     <row r="35" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="4" t="str">

</xml_diff>